<commit_message>
custom excel reports. crud profiles, users. various fixes.
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/reportTemplate.xlsx
+++ b/src/main/resources/templates/excel/reportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\Projects\framework-showcase\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D591F1C2-3A44-4039-851F-442672F54642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C3AE5-4CB7-41A7-B40A-40BA185B864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,11 +35,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabriel Marte</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3918FC09-6FD1-4A37-A6F4-FB9F13F38C2D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:area(sheetStreaming="true" lastCell="Z7")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{1C200B1E-1EDA-4392-BA20-7B237FE92C43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:each(items="data" var="it" lastCell="Z7")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>${creationDate}</t>
   </si>
@@ -63,9 +98,6 @@
   </si>
   <si>
     <t>${range}</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${data}" var="it"&gt;</t>
   </si>
   <si>
     <t>${it.word}</t>
@@ -85,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -113,13 +145,6 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
@@ -132,6 +157,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -215,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,29 +255,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -528,8 +556,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -546,19 +574,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
+      <c r="A2" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -568,8 +596,8 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>3</v>
+      <c r="A3" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -579,59 +607,43 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>8</v>
+      <c r="A4" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -639,5 +651,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>